<commit_message>
fix(db, seeders), doc(standardization files name)
Correction de la db, seeders. Gestion des seeders;

Correction des noms des fichiers doc/ , unifing-standartizing
</commit_message>
<xml_diff>
--- a/Doc/TEST-Journal-de-Travail_NademoYosef.xlsx
+++ b/Doc/TEST-Journal-de-Travail_NademoYosef.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\cicd-todo-app\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1813C6C-94E4-44BE-B19A-4720AFF200C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC652E8C-9BAA-4CA5-B668-52DD08443AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6555" yWindow="0" windowWidth="21600" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="6555" yWindow="1020" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>Auteur:</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>resolution des problemese de versioning</t>
+  </si>
+  <si>
+    <t>Correction de la db, seeders. Gestion des seeders</t>
+  </si>
+  <si>
+    <t>correction des noms des fichiers doc/ , unifing-standartizing</t>
   </si>
 </sst>
 </file>
@@ -1235,13 +1241,13 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>365</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2165,16 +2171,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.15686274509803921</c:v>
+                  <c:v>0.14814814814814814</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12745098039215685</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.71568627450980393</c:v>
+                  <c:v>0.68518518518518523</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4363,7 +4369,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4418,7 +4424,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>8 heures 30 minutes</v>
+        <v>9 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4437,11 +4443,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>450</v>
+        <v>480</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>510</v>
+        <v>540</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5057,35 +5063,53 @@
       <c r="G31" s="84"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="62" t="str">
+      <c r="A32" s="62">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B32))</f>
-        <v/>
-      </c>
-      <c r="B32" s="30"/>
+        <v>49</v>
+      </c>
+      <c r="B32" s="30">
+        <v>45995</v>
+      </c>
       <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="23"/>
+      <c r="D32" s="32">
+        <v>25</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>56</v>
+      </c>
       <c r="G32" s="39"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="63" t="str">
+      <c r="A33" s="63">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B33))</f>
-        <v/>
-      </c>
-      <c r="B33" s="34"/>
+        <v>49</v>
+      </c>
+      <c r="B33" s="34">
+        <v>45995</v>
+      </c>
       <c r="C33" s="35"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="22"/>
+      <c r="D33" s="36">
+        <v>5</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>57</v>
+      </c>
       <c r="G33" s="40"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="62" t="str">
+      <c r="A34" s="62">
         <f>IF(ISBLANK(B34),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B34))</f>
-        <v/>
-      </c>
-      <c r="B34" s="30"/>
+        <v>49</v>
+      </c>
+      <c r="B34" s="30">
+        <v>45995</v>
+      </c>
       <c r="C34" s="31"/>
       <c r="D34" s="32"/>
       <c r="E34" s="33"/>
@@ -5093,11 +5117,13 @@
       <c r="G34" s="39"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="63" t="str">
+      <c r="A35" s="63">
         <f>IF(ISBLANK(B35),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B35))</f>
-        <v/>
-      </c>
-      <c r="B35" s="34"/>
+        <v>49</v>
+      </c>
+      <c r="B35" s="34">
+        <v>45995</v>
+      </c>
       <c r="C35" s="35"/>
       <c r="D35" s="36"/>
       <c r="E35" s="37"/>
@@ -5105,11 +5131,13 @@
       <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="62" t="str">
+      <c r="A36" s="62">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B36))</f>
-        <v/>
-      </c>
-      <c r="B36" s="30"/>
+        <v>49</v>
+      </c>
+      <c r="B36" s="30">
+        <v>45995</v>
+      </c>
       <c r="C36" s="31"/>
       <c r="D36" s="32"/>
       <c r="E36" s="33"/>
@@ -5117,11 +5145,13 @@
       <c r="G36" s="39"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="63" t="str">
+      <c r="A37" s="63">
         <f>IF(ISBLANK(B37),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B37))</f>
-        <v/>
-      </c>
-      <c r="B37" s="34"/>
+        <v>49</v>
+      </c>
+      <c r="B37" s="34">
+        <v>45995</v>
+      </c>
       <c r="C37" s="35"/>
       <c r="D37" s="36"/>
       <c r="E37" s="37"/>
@@ -11234,7 +11264,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.15686274509803921</v>
+        <v>0.14814814814814814</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11255,11 +11285,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11267,11 +11297,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>1 h 05 min</v>
+        <v>1 h 30 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.12745098039215685</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11329,11 +11359,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11341,11 +11371,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>6 h 05 min</v>
+        <v>6 h 10 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.71568627450980393</v>
+        <v>0.68518518518518523</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11401,22 +11431,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>450</v>
+        <v>480</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>510</v>
+        <v>540</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>8 h 30 min</v>
+        <v>9 h 00 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.35416666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
feat(deploy script, added seeders)
</commit_message>
<xml_diff>
--- a/Doc/TEST-Journal-de-Travail_NademoYosef.xlsx
+++ b/Doc/TEST-Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\cicd-todo-app\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC652E8C-9BAA-4CA5-B668-52DD08443AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE45C754-673F-40AC-8046-E770B997EC6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6555" yWindow="1020" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
   <si>
     <t>Auteur:</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>correction des noms des fichiers doc/ , unifing-standartizing</t>
+  </si>
+  <si>
+    <t>fix(.env error sloved), feat(better deploy script) + added seeders</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1244,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2171,16 +2174,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.14814814814814814</c:v>
+                  <c:v>0.1415929203539823</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.20353982300884957</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.68518518518518523</c:v>
+                  <c:v>0.65486725663716816</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4369,7 +4372,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4424,7 +4427,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>9 heures 0 minutes</v>
+        <v>9 heures 25 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4443,11 +4446,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>480</v>
+        <v>505</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>540</v>
+        <v>565</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5111,9 +5114,15 @@
         <v>45995</v>
       </c>
       <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="22"/>
+      <c r="D34" s="32">
+        <v>25</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="G34" s="39"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -11264,7 +11273,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.14814814814814814</v>
+        <v>0.1415929203539823</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11285,11 +11294,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11297,11 +11306,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>1 h 30 min</v>
+        <v>1 h 55 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.16666666666666666</v>
+        <v>0.20353982300884957</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11375,7 +11384,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.68518518518518523</v>
+        <v>0.65486725663716816</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11431,22 +11440,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>480</v>
+        <v>505</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>540</v>
+        <v>565</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>9 h 00 min</v>
+        <v>9 h 25 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.375</v>
+        <v>0.3923611111111111</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11490,15 +11499,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11507,6 +11507,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11711,14 +11720,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11727,6 +11728,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
doc(plan de tests corrigé)
</commit_message>
<xml_diff>
--- a/Doc/TEST-Journal-de-Travail_NademoYosef.xlsx
+++ b/Doc/TEST-Journal-de-Travail_NademoYosef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pn25kdv\Documents\GitHub\cicd-todo-app\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE45C754-673F-40AC-8046-E770B997EC6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABC77AC-723E-4CC6-80A2-4C8EBD297992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6555" yWindow="1020" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>Auteur:</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>fix(.env error sloved), feat(better deploy script) + added seeders</t>
+  </si>
+  <si>
+    <t>plan de tests corrigé</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1253,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>370</c:v>
+                  <c:v>380</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2174,16 +2177,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.1415929203539823</c:v>
+                  <c:v>0.1391304347826087</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20353982300884957</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65486725663716816</c:v>
+                  <c:v>0.66086956521739126</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4372,7 +4375,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4427,7 +4430,7 @@
       <c r="B3" s="88"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>9 heures 25 minutes</v>
+        <v>9 heures 35 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4446,11 +4449,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>505</v>
+        <v>515</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>565</v>
+        <v>575</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5134,9 +5137,15 @@
         <v>45995</v>
       </c>
       <c r="C35" s="35"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="23"/>
+      <c r="D35" s="36">
+        <v>10</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -11273,7 +11282,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.1415929203539823</v>
+        <v>0.1391304347826087</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11310,7 +11319,7 @@
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.20353982300884957</v>
+        <v>0.2</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11368,11 +11377,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11380,11 +11389,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>6 h 10 min</v>
+        <v>6 h 20 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.65486725663716816</v>
+        <v>0.66086956521739126</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11440,22 +11449,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>505</v>
+        <v>515</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>565</v>
+        <v>575</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>9 h 25 min</v>
+        <v>9 h 35 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.3923611111111111</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11499,6 +11508,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11507,15 +11525,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11720,6 +11729,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11728,14 +11745,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>